<commit_message>
Updated status for 7th April-pratiksha,me and gautami
</commit_message>
<xml_diff>
--- a/Daily Status update Report 07042020.xlsx
+++ b/Daily Status update Report 07042020.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="11"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="124">
   <si>
     <t>Employee Name</t>
   </si>
@@ -393,13 +393,22 @@
   </si>
   <si>
     <t>Going through the Interface Flow diagram; preparing points for meeting with mentees on PT SLA</t>
+  </si>
+  <si>
+    <t>Completed with Test Cases Writing for Collateral Withdraw Cash - Checked-Checked-Margin Deposit Scenario(for Created-&gt;Accepted-&gt; Settled)</t>
+  </si>
+  <si>
+    <t>Understanding SLA document and Interface service flow; working on cucumber</t>
+  </si>
+  <si>
+    <t>Working on keyword driven framework</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -563,6 +572,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,21 +845,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -860,7 +870,7 @@
     <col min="7" max="7" width="117.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -883,7 +893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -906,7 +916,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -929,7 +939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -952,7 +962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -975,7 +985,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -998,7 +1008,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1021,7 +1031,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1044,7 +1054,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1067,7 +1077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1090,7 +1100,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1113,7 +1123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1134,7 +1144,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1162,14 +1172,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1180,7 +1190,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1203,7 +1213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1226,7 +1236,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1249,7 +1259,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1272,7 +1282,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1295,7 +1305,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1318,7 +1328,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1341,7 +1351,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1364,7 +1374,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1387,7 +1397,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1410,7 +1420,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1433,7 +1443,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1456,7 +1466,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -1479,7 +1489,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1509,14 +1519,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G12" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1527,7 +1537,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1550,7 +1560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1571,7 +1581,7 @@
       </c>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1592,7 +1602,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1613,7 +1623,7 @@
       </c>
       <c r="G4" s="31"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1634,7 +1644,7 @@
       </c>
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1655,7 +1665,7 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1676,7 +1686,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1697,7 +1707,7 @@
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1718,7 +1728,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1741,7 +1751,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1764,7 +1774,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1787,7 +1797,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -1810,7 +1820,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1838,14 +1848,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1856,7 +1866,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1879,7 +1889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1900,7 +1910,7 @@
       </c>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1921,7 +1931,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1942,7 +1952,7 @@
       </c>
       <c r="G4" s="31"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1963,7 +1973,7 @@
       </c>
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1984,7 +1994,7 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2005,7 +2015,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2026,7 +2036,7 @@
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2047,7 +2057,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -2070,7 +2080,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -2089,9 +2099,11 @@
       <c r="F11" s="34">
         <v>0.75</v>
       </c>
-      <c r="G11" s="32"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -2110,9 +2122,11 @@
       <c r="F12" s="34">
         <v>0.75</v>
       </c>
-      <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -2131,9 +2145,11 @@
       <c r="F13" s="34">
         <v>0.75</v>
       </c>
-      <c r="G13" s="32"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -2156,18 +2172,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2178,7 +2195,7 @@
     <col min="7" max="7" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2201,7 +2218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2224,7 +2241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2247,7 +2264,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2270,7 +2287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2293,7 +2310,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2316,7 +2333,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2339,7 +2356,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2362,7 +2379,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2385,7 +2402,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2408,7 +2425,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2431,7 +2448,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2454,7 +2471,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2484,14 +2501,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2502,7 +2519,7 @@
     <col min="7" max="7" width="136.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2525,7 +2542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2548,7 +2565,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2571,7 +2588,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2594,7 +2611,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2617,7 +2634,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2640,7 +2657,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2663,7 +2680,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2686,7 +2703,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2709,7 +2726,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2732,7 +2749,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2755,7 +2772,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2778,7 +2795,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2808,14 +2825,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2826,7 +2843,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2849,7 +2866,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2872,7 +2889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2895,7 +2912,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2918,7 +2935,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2941,7 +2958,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2964,7 +2981,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2987,7 +3004,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3010,7 +3027,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3033,7 +3050,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3056,7 +3073,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3079,7 +3096,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3102,7 +3119,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3125,7 +3142,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3155,14 +3172,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3173,7 +3190,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3196,7 +3213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3219,7 +3236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3242,7 +3259,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3265,7 +3282,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3288,7 +3305,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3311,7 +3328,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3334,7 +3351,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3357,7 +3374,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3380,7 +3397,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3403,7 +3420,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3426,7 +3443,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3449,7 +3466,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3472,7 +3489,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3502,14 +3519,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3520,7 +3537,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3543,7 +3560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3566,7 +3583,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3589,7 +3606,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3612,7 +3629,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3635,7 +3652,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3658,7 +3675,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3681,7 +3698,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3704,7 +3721,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3727,7 +3744,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3750,7 +3767,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3773,7 +3790,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3796,7 +3813,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3819,7 +3836,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3849,14 +3866,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3867,7 +3884,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3890,7 +3907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3913,7 +3930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3936,7 +3953,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3959,7 +3976,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3982,7 +3999,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4005,7 +4022,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4028,7 +4045,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4051,7 +4068,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4074,7 +4091,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -4097,7 +4114,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -4120,7 +4137,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4143,7 +4160,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -4166,7 +4183,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -4196,14 +4213,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -4214,7 +4231,7 @@
     <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
@@ -4237,7 +4254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -4260,7 +4277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -4283,7 +4300,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -4306,7 +4323,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -4329,7 +4346,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -4352,7 +4369,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -4375,7 +4392,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -4398,7 +4415,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -4421,7 +4438,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -4444,7 +4461,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -4467,7 +4484,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -4490,7 +4507,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -4513,7 +4530,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -4543,14 +4560,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -4561,7 +4578,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4584,7 +4601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4607,7 +4624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4630,7 +4647,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4653,7 +4670,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4676,7 +4693,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4699,7 +4716,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4722,7 +4739,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4745,7 +4762,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4768,7 +4785,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -4791,7 +4808,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -4814,7 +4831,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -4837,7 +4854,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -4860,7 +4877,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Updated status for 8th April- Pratiksha,Me and Gautami
</commit_message>
<xml_diff>
--- a/Daily Status update Report 07042020.xlsx
+++ b/Daily Status update Report 07042020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="138">
   <si>
     <t>Sr.No</t>
   </si>
@@ -435,12 +435,18 @@
   <si>
     <t>Team Discussion and Use case document understanding for Collateral and Settlement</t>
   </si>
+  <si>
+    <t>Completed with Test Cases Writing for Collateral Withdraw Cash - Checked-Checked-Margin Deposit Scenario(for Created-&gt;Accepted-&gt;Manually Settled); Understanding Modified Trade Flow for Rectify Quantiy</t>
+  </si>
+  <si>
+    <t>Discussion on SLA document for PT; Working on cucumber</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,6 +475,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -532,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -622,6 +635,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2138,8 +2155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -4794,7 +4811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -6121,7 +6140,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -6348,7 +6369,7 @@
       </c>
       <c r="G10" s="29"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -6367,7 +6388,9 @@
       <c r="F11" s="31">
         <v>0.75</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="35" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="9">
@@ -6388,7 +6411,9 @@
       <c r="F12" s="31">
         <v>0.75</v>
       </c>
-      <c r="G12" s="29"/>
+      <c r="G12" s="36" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="9">
@@ -6409,7 +6434,9 @@
       <c r="F13" s="31">
         <v>0.75</v>
       </c>
-      <c r="G13" s="29"/>
+      <c r="G13" s="29" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="9">
@@ -6434,6 +6461,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
status updated for 8th april
</commit_message>
<xml_diff>
--- a/Daily Status update Report 07042020.xlsx
+++ b/Daily Status update Report 07042020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="137">
   <si>
     <t>Sr.No</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>Team Discussion and Use case document understanding for Collateral and Settlement</t>
+  </si>
+  <si>
+    <t>Working on keyword driven framework;</t>
   </si>
 </sst>
 </file>
@@ -6121,7 +6124,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -6409,7 +6414,9 @@
       <c r="F13" s="31">
         <v>0.75</v>
       </c>
-      <c r="G13" s="29"/>
+      <c r="G13" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="9">

</xml_diff>